<commit_message>
fix template strings not supported in IE 11
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Epi-X-Format.xlsx
+++ b/test/fixtures/files/Epi-X-Format.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aholmes/Developer/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A77CCC4-F18B-F844-9A61-B35B6B9DFEB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92ED9AB9-8A75-834C-AFBC-BB734C401983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2580" yWindow="2140" windowWidth="28800" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="200">
   <si>
     <t>DGMQ ID</t>
   </si>
@@ -617,6 +617,9 @@
   </si>
   <si>
     <t>EX-3a9212</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1449,7 @@
   <dimension ref="A1:BC12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2021,7 +2024,7 @@
         <v>36331</v>
       </c>
       <c r="N7" t="s">
-        <v>97</v>
+        <v>199</v>
       </c>
       <c r="Q7" t="s">
         <v>139</v>
@@ -2138,9 +2141,6 @@
       </c>
       <c r="M9" s="3">
         <v>20142</v>
-      </c>
-      <c r="N9" t="s">
-        <v>97</v>
       </c>
       <c r="Q9" t="s">
         <v>160</v>

</xml_diff>

<commit_message>
Update Epi-X test file to have valid dates
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Epi-X-Format.xlsx
+++ b/test/fixtures/files/Epi-X-Format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kfagan/Documents/Projects/CDC/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92ED9AB9-8A75-834C-AFBC-BB734C401983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073F08AA-064C-334F-9C5A-EF3F05C629C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2580" yWindow="2140" windowWidth="28800" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="199">
   <si>
     <t>DGMQ ID</t>
   </si>
@@ -577,15 +577,9 @@
     <t>Vermont</t>
   </si>
   <si>
-    <t>2019-11-19</t>
-  </si>
-  <si>
     <t>2020-01-06</t>
   </si>
   <si>
-    <t>2019-12-31</t>
-  </si>
-  <si>
     <t>1965-09-08</t>
   </si>
   <si>
@@ -620,6 +614,9 @@
   </si>
   <si>
     <t>U</t>
+  </si>
+  <si>
+    <t>2020-01-01</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1446,7 @@
   <dimension ref="A1:BC12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1668,7 +1665,7 @@
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
         <v>62</v>
@@ -1729,18 +1726,18 @@
         <v>55</v>
       </c>
       <c r="AK2" s="3">
-        <v>43829</v>
+        <v>43983</v>
       </c>
       <c r="AP2" t="s">
         <v>170</v>
       </c>
       <c r="AQ2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -1809,7 +1806,7 @@
         <v>71</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J4" t="s">
         <v>77</v>
@@ -1861,7 +1858,7 @@
       </c>
       <c r="AK4" s="3"/>
       <c r="AP4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.2">
@@ -1876,7 +1873,7 @@
         <v>1842</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="J5" t="s">
         <v>78</v>
@@ -1921,7 +1918,7 @@
         <v>43892</v>
       </c>
       <c r="AQ5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.2">
@@ -1939,7 +1936,7 @@
         <v>72</v>
       </c>
       <c r="I6" s="3">
-        <v>43788</v>
+        <v>44141</v>
       </c>
       <c r="J6" t="s">
         <v>79</v>
@@ -1981,10 +1978,10 @@
         <v>154</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AE6" s="6" t="s">
         <v>115</v>
@@ -1993,8 +1990,8 @@
       <c r="AJ6" t="s">
         <v>121</v>
       </c>
-      <c r="AK6" s="5" t="s">
-        <v>185</v>
+      <c r="AK6" s="3">
+        <v>43831</v>
       </c>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.2">
@@ -2009,7 +2006,7 @@
         <v>1242</v>
       </c>
       <c r="I7" s="3">
-        <v>43828</v>
+        <v>43894</v>
       </c>
       <c r="J7" t="s">
         <v>80</v>
@@ -2024,7 +2021,7 @@
         <v>36331</v>
       </c>
       <c r="N7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="Q7" t="s">
         <v>139</v>
@@ -2048,7 +2045,7 @@
         <v>116</v>
       </c>
       <c r="AP7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.2">
@@ -2111,7 +2108,7 @@
         <v>43895</v>
       </c>
       <c r="AQ8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.2">
@@ -2176,7 +2173,7 @@
         <v>123</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="N10" t="s">
         <v>60</v>
@@ -2209,7 +2206,7 @@
         <v>166</v>
       </c>
       <c r="AP10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.2">

</xml_diff>